<commit_message>
Last commit before handing in lab 3
</commit_message>
<xml_diff>
--- a/Lab 3/rectifier data.xlsx
+++ b/Lab 3/rectifier data.xlsx
@@ -111,9 +111,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,10 +667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="A1:F7"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,9 +679,10 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -698,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -715,8 +719,9 @@
         <f>C2/B2</f>
         <v>2.6755852842809364E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -736,8 +741,9 @@
         <f>C3/B3</f>
         <v>9.7165991902834009E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -757,8 +763,9 @@
         <f t="shared" ref="F4:F7" si="0">C4/B4</f>
         <v>0.10344827586206896</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -778,8 +785,9 @@
         <f t="shared" si="0"/>
         <v>0.12755102040816327</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -799,8 +807,9 @@
         <f t="shared" si="0"/>
         <v>0.11552346570397112</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -820,8 +829,14 @@
         <f t="shared" si="0"/>
         <v>0.1079136690647482</v>
       </c>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G6:G7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -829,10 +844,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="A1:F5"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,9 +857,10 @@
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -864,7 +880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -884,8 +900,9 @@
         <f>C2/B2</f>
         <v>7.6335877862595426E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -905,8 +922,9 @@
         <f>C3/B3</f>
         <v>8.1967213114754103E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -926,8 +944,9 @@
         <f t="shared" ref="F4:F5" si="0">C4/B4</f>
         <v>3.3898305084745763E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -947,8 +966,14 @@
         <f t="shared" si="0"/>
         <v>7.9365079365079378E-3</v>
       </c>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>